<commit_message>
Misc Clean up - final upload by me hopefully
Made demand analysis dp consistent
Re-ran sim for the slack histograms
removed deprecated simulation.py
</commit_message>
<xml_diff>
--- a/DemandAnalysis.xlsx
+++ b/DemandAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lara\Documents\GitHub\263-OR-18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D305AA71-A5FC-474C-B540-9BB582CBCC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235B159F-EE02-4C82-A623-08A104FFA4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32835" yWindow="-225" windowWidth="18600" windowHeight="8955" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35535" yWindow="4410" windowWidth="18600" windowHeight="8955" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Saturdays" sheetId="1" r:id="rId1"/>
@@ -760,13 +760,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1126,7 +1125,7 @@
   <dimension ref="A1:V56"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+      <selection activeCell="O2" sqref="O2:T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3946,6 +3945,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3954,7 +3954,7 @@
   <dimension ref="A1:AH66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AH6" sqref="AH6"/>
+      <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4089,51 +4089,51 @@
         <v>7</v>
       </c>
       <c r="V2">
-        <f>AVERAGE(A2:U2)</f>
+        <f t="shared" ref="V2:V33" si="0">AVERAGE(A2:U2)</f>
         <v>7.1</v>
       </c>
       <c r="W2">
-        <f>_xlfn.CEILING.MATH(V2)</f>
+        <f t="shared" ref="W2:W33" si="1">_xlfn.CEILING.MATH(V2)</f>
         <v>8</v>
       </c>
       <c r="X2">
-        <f>COUNTIF(B2:U2,"&lt;"&amp;V2)/COUNT(B2:U2)*100</f>
+        <f t="shared" ref="X2:X33" si="2">COUNTIF(B2:U2,"&lt;"&amp;V2)/COUNT(B2:U2)*100</f>
         <v>60</v>
       </c>
       <c r="Y2">
-        <f>COUNTIF(B2:U2,"&gt;"&amp;V2)/COUNT(B2:U2)*100</f>
+        <f t="shared" ref="Y2:Y33" si="3">COUNTIF(B2:U2,"&gt;"&amp;V2)/COUNT(B2:U2)*100</f>
         <v>40</v>
       </c>
       <c r="Z2">
-        <f>COUNTIF(B2:U2,"&lt;"&amp;W2)/COUNT(B2:U2)*100</f>
+        <f t="shared" ref="Z2:Z33" si="4">COUNTIF(B2:U2,"&lt;"&amp;W2)/COUNT(B2:U2)*100</f>
         <v>60</v>
       </c>
       <c r="AA2">
-        <f>COUNTIF(B2:U2,"&gt;"&amp;U2)/COUNT(B2:U2)*100</f>
+        <f t="shared" ref="AA2:AA33" si="5">COUNTIF(B2:U2,"&gt;"&amp;U2)/COUNT(B2:U2)*100</f>
         <v>40</v>
       </c>
-      <c r="AC2" s="5">
-        <f>AVERAGE(V:V)</f>
+      <c r="AC2" s="2">
+        <f t="shared" ref="AC2:AH2" si="6">AVERAGE(V:V)</f>
         <v>7.3269230769230758</v>
       </c>
-      <c r="AD2" s="5">
-        <f>AVERAGE(W:W)</f>
+      <c r="AD2" s="2">
+        <f t="shared" si="6"/>
         <v>7.8307692307692305</v>
       </c>
-      <c r="AE2" s="5">
-        <f>AVERAGE(X:X)</f>
+      <c r="AE2" s="2">
+        <f t="shared" si="6"/>
         <v>50.92307692307692</v>
       </c>
-      <c r="AF2" s="5">
-        <f>AVERAGE(Y:Y)</f>
+      <c r="AF2" s="2">
+        <f t="shared" si="6"/>
         <v>48.153846153846153</v>
       </c>
-      <c r="AG2" s="5">
-        <f>AVERAGE(Z:Z)</f>
+      <c r="AG2" s="2">
+        <f t="shared" si="6"/>
         <v>50.92307692307692</v>
       </c>
-      <c r="AH2" s="5">
-        <f>AVERAGE(AA:AA)</f>
+      <c r="AH2" s="2">
+        <f t="shared" si="6"/>
         <v>41.307692307692307</v>
       </c>
     </row>
@@ -4202,27 +4202,27 @@
         <v>5</v>
       </c>
       <c r="V3">
-        <f>AVERAGE(A3:U3)</f>
+        <f t="shared" si="0"/>
         <v>8.0500000000000007</v>
       </c>
       <c r="W3">
-        <f>_xlfn.CEILING.MATH(V3)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X3">
-        <f>COUNTIF(B3:U3,"&lt;"&amp;V3)/COUNT(B3:U3)*100</f>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="Y3">
-        <f>COUNTIF(B3:U3,"&gt;"&amp;V3)/COUNT(B3:U3)*100</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="Z3">
-        <f>COUNTIF(B3:U3,"&lt;"&amp;W3)/COUNT(B3:U3)*100</f>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="AA3">
-        <f>COUNTIF(B3:U3,"&gt;"&amp;U3)/COUNT(B3:U3)*100</f>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
     </row>
@@ -4291,27 +4291,27 @@
         <v>9</v>
       </c>
       <c r="V4">
-        <f>AVERAGE(A4:U4)</f>
+        <f t="shared" si="0"/>
         <v>7.7</v>
       </c>
       <c r="W4">
-        <f>_xlfn.CEILING.MATH(V4)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="X4">
-        <f>COUNTIF(B4:U4,"&lt;"&amp;V4)/COUNT(B4:U4)*100</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="Y4">
-        <f>COUNTIF(B4:U4,"&gt;"&amp;V4)/COUNT(B4:U4)*100</f>
+        <f t="shared" si="3"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Z4">
-        <f>COUNTIF(B4:U4,"&lt;"&amp;W4)/COUNT(B4:U4)*100</f>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="AA4">
-        <f>COUNTIF(B4:U4,"&gt;"&amp;U4)/COUNT(B4:U4)*100</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
     </row>
@@ -4380,27 +4380,27 @@
         <v>12</v>
       </c>
       <c r="V5">
-        <f>AVERAGE(A5:U5)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="W5">
-        <f>_xlfn.CEILING.MATH(V5)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="X5">
-        <f>COUNTIF(B5:U5,"&lt;"&amp;V5)/COUNT(B5:U5)*100</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="Y5">
-        <f>COUNTIF(B5:U5,"&gt;"&amp;V5)/COUNT(B5:U5)*100</f>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="Z5">
-        <f>COUNTIF(B5:U5,"&lt;"&amp;W5)/COUNT(B5:U5)*100</f>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="AA5">
-        <f>COUNTIF(B5:U5,"&gt;"&amp;U5)/COUNT(B5:U5)*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4469,27 +4469,27 @@
         <v>3</v>
       </c>
       <c r="V6">
-        <f>AVERAGE(A6:U6)</f>
+        <f t="shared" si="0"/>
         <v>7.2</v>
       </c>
       <c r="W6">
-        <f>_xlfn.CEILING.MATH(V6)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="X6">
-        <f>COUNTIF(B6:U6,"&lt;"&amp;V6)/COUNT(B6:U6)*100</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="Y6">
-        <f>COUNTIF(B6:U6,"&gt;"&amp;V6)/COUNT(B6:U6)*100</f>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="Z6">
-        <f>COUNTIF(B6:U6,"&lt;"&amp;W6)/COUNT(B6:U6)*100</f>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="AA6">
-        <f>COUNTIF(B6:U6,"&gt;"&amp;U6)/COUNT(B6:U6)*100</f>
+        <f t="shared" si="5"/>
         <v>95</v>
       </c>
     </row>
@@ -4558,27 +4558,27 @@
         <v>4</v>
       </c>
       <c r="V7">
-        <f>AVERAGE(A7:U7)</f>
+        <f t="shared" si="0"/>
         <v>8.1999999999999993</v>
       </c>
       <c r="W7">
-        <f>_xlfn.CEILING.MATH(V7)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X7">
-        <f>COUNTIF(B7:U7,"&lt;"&amp;V7)/COUNT(B7:U7)*100</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="Y7">
-        <f>COUNTIF(B7:U7,"&gt;"&amp;V7)/COUNT(B7:U7)*100</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="Z7">
-        <f>COUNTIF(B7:U7,"&lt;"&amp;W7)/COUNT(B7:U7)*100</f>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="AA7">
-        <f>COUNTIF(B7:U7,"&gt;"&amp;U7)/COUNT(B7:U7)*100</f>
+        <f t="shared" si="5"/>
         <v>95</v>
       </c>
     </row>
@@ -4647,27 +4647,27 @@
         <v>9</v>
       </c>
       <c r="V8">
-        <f>AVERAGE(A8:U8)</f>
+        <f t="shared" si="0"/>
         <v>8.15</v>
       </c>
       <c r="W8">
-        <f>_xlfn.CEILING.MATH(V8)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X8">
-        <f>COUNTIF(B8:U8,"&lt;"&amp;V8)/COUNT(B8:U8)*100</f>
+        <f t="shared" si="2"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Y8">
-        <f>COUNTIF(B8:U8,"&gt;"&amp;V8)/COUNT(B8:U8)*100</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="Z8">
-        <f>COUNTIF(B8:U8,"&lt;"&amp;W8)/COUNT(B8:U8)*100</f>
+        <f t="shared" si="4"/>
         <v>55.000000000000007</v>
       </c>
       <c r="AA8">
-        <f>COUNTIF(B8:U8,"&gt;"&amp;U8)/COUNT(B8:U8)*100</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
     </row>
@@ -4736,27 +4736,27 @@
         <v>6</v>
       </c>
       <c r="V9">
-        <f>AVERAGE(A9:U9)</f>
+        <f t="shared" si="0"/>
         <v>7.05</v>
       </c>
       <c r="W9">
-        <f>_xlfn.CEILING.MATH(V9)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="X9">
-        <f>COUNTIF(B9:U9,"&lt;"&amp;V9)/COUNT(B9:U9)*100</f>
+        <f t="shared" si="2"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Y9">
-        <f>COUNTIF(B9:U9,"&gt;"&amp;V9)/COUNT(B9:U9)*100</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="Z9">
-        <f>COUNTIF(B9:U9,"&lt;"&amp;W9)/COUNT(B9:U9)*100</f>
+        <f t="shared" si="4"/>
         <v>55.000000000000007</v>
       </c>
       <c r="AA9">
-        <f>COUNTIF(B9:U9,"&gt;"&amp;U9)/COUNT(B9:U9)*100</f>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
     </row>
@@ -4825,27 +4825,27 @@
         <v>5</v>
       </c>
       <c r="V10">
-        <f>AVERAGE(A10:U10)</f>
+        <f t="shared" si="0"/>
         <v>8.35</v>
       </c>
       <c r="W10">
-        <f>_xlfn.CEILING.MATH(V10)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X10">
-        <f>COUNTIF(B10:U10,"&lt;"&amp;V10)/COUNT(B10:U10)*100</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="Y10">
-        <f>COUNTIF(B10:U10,"&gt;"&amp;V10)/COUNT(B10:U10)*100</f>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="Z10">
-        <f>COUNTIF(B10:U10,"&lt;"&amp;W10)/COUNT(B10:U10)*100</f>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="AA10">
-        <f>COUNTIF(B10:U10,"&gt;"&amp;U10)/COUNT(B10:U10)*100</f>
+        <f t="shared" si="5"/>
         <v>80</v>
       </c>
     </row>
@@ -4914,27 +4914,27 @@
         <v>11</v>
       </c>
       <c r="V11">
-        <f>AVERAGE(A11:U11)</f>
+        <f t="shared" si="0"/>
         <v>8.6</v>
       </c>
       <c r="W11">
-        <f>_xlfn.CEILING.MATH(V11)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X11">
-        <f>COUNTIF(B11:U11,"&lt;"&amp;V11)/COUNT(B11:U11)*100</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="Y11">
-        <f>COUNTIF(B11:U11,"&gt;"&amp;V11)/COUNT(B11:U11)*100</f>
+        <f t="shared" si="3"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Z11">
-        <f>COUNTIF(B11:U11,"&lt;"&amp;W11)/COUNT(B11:U11)*100</f>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="AA11">
-        <f>COUNTIF(B11:U11,"&gt;"&amp;U11)/COUNT(B11:U11)*100</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
@@ -5003,27 +5003,27 @@
         <v>7</v>
       </c>
       <c r="V12">
-        <f>AVERAGE(A12:U12)</f>
+        <f t="shared" si="0"/>
         <v>8.3000000000000007</v>
       </c>
       <c r="W12">
-        <f>_xlfn.CEILING.MATH(V12)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X12">
-        <f>COUNTIF(B12:U12,"&lt;"&amp;V12)/COUNT(B12:U12)*100</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="Y12">
-        <f>COUNTIF(B12:U12,"&gt;"&amp;V12)/COUNT(B12:U12)*100</f>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="Z12">
-        <f>COUNTIF(B12:U12,"&lt;"&amp;W12)/COUNT(B12:U12)*100</f>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="AA12">
-        <f>COUNTIF(B12:U12,"&gt;"&amp;U12)/COUNT(B12:U12)*100</f>
+        <f t="shared" si="5"/>
         <v>55.000000000000007</v>
       </c>
     </row>
@@ -5092,27 +5092,27 @@
         <v>3</v>
       </c>
       <c r="V13">
-        <f>AVERAGE(A13:U13)</f>
+        <f t="shared" si="0"/>
         <v>7.3</v>
       </c>
       <c r="W13">
-        <f>_xlfn.CEILING.MATH(V13)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="X13">
-        <f>COUNTIF(B13:U13,"&lt;"&amp;V13)/COUNT(B13:U13)*100</f>
+        <f t="shared" si="2"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Y13">
-        <f>COUNTIF(B13:U13,"&gt;"&amp;V13)/COUNT(B13:U13)*100</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="Z13">
-        <f>COUNTIF(B13:U13,"&lt;"&amp;W13)/COUNT(B13:U13)*100</f>
+        <f t="shared" si="4"/>
         <v>55.000000000000007</v>
       </c>
       <c r="AA13">
-        <f>COUNTIF(B13:U13,"&gt;"&amp;U13)/COUNT(B13:U13)*100</f>
+        <f t="shared" si="5"/>
         <v>95</v>
       </c>
     </row>
@@ -5181,27 +5181,27 @@
         <v>12</v>
       </c>
       <c r="V14">
-        <f>AVERAGE(A14:U14)</f>
+        <f t="shared" si="0"/>
         <v>7.9</v>
       </c>
       <c r="W14">
-        <f>_xlfn.CEILING.MATH(V14)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="X14">
-        <f>COUNTIF(B14:U14,"&lt;"&amp;V14)/COUNT(B14:U14)*100</f>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="Y14">
-        <f>COUNTIF(B14:U14,"&gt;"&amp;V14)/COUNT(B14:U14)*100</f>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="Z14">
-        <f>COUNTIF(B14:U14,"&lt;"&amp;W14)/COUNT(B14:U14)*100</f>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="AA14">
-        <f>COUNTIF(B14:U14,"&gt;"&amp;U14)/COUNT(B14:U14)*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5270,27 +5270,27 @@
         <v>5</v>
       </c>
       <c r="V15">
-        <f>AVERAGE(A15:U15)</f>
+        <f t="shared" si="0"/>
         <v>7.65</v>
       </c>
       <c r="W15">
-        <f>_xlfn.CEILING.MATH(V15)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="X15">
-        <f>COUNTIF(B15:U15,"&lt;"&amp;V15)/COUNT(B15:U15)*100</f>
+        <f t="shared" si="2"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Y15">
-        <f>COUNTIF(B15:U15,"&gt;"&amp;V15)/COUNT(B15:U15)*100</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="Z15">
-        <f>COUNTIF(B15:U15,"&lt;"&amp;W15)/COUNT(B15:U15)*100</f>
+        <f t="shared" si="4"/>
         <v>55.000000000000007</v>
       </c>
       <c r="AA15">
-        <f>COUNTIF(B15:U15,"&gt;"&amp;U15)/COUNT(B15:U15)*100</f>
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
     </row>
@@ -5359,27 +5359,27 @@
         <v>5</v>
       </c>
       <c r="V16">
-        <f>AVERAGE(A16:U16)</f>
+        <f t="shared" si="0"/>
         <v>8.6</v>
       </c>
       <c r="W16">
-        <f>_xlfn.CEILING.MATH(V16)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X16">
-        <f>COUNTIF(B16:U16,"&lt;"&amp;V16)/COUNT(B16:U16)*100</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="Y16">
-        <f>COUNTIF(B16:U16,"&gt;"&amp;V16)/COUNT(B16:U16)*100</f>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="Z16">
-        <f>COUNTIF(B16:U16,"&lt;"&amp;W16)/COUNT(B16:U16)*100</f>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="AA16">
-        <f>COUNTIF(B16:U16,"&gt;"&amp;U16)/COUNT(B16:U16)*100</f>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
     </row>
@@ -5448,27 +5448,27 @@
         <v>9</v>
       </c>
       <c r="V17">
-        <f>AVERAGE(A17:U17)</f>
+        <f t="shared" si="0"/>
         <v>8.9499999999999993</v>
       </c>
       <c r="W17">
-        <f>_xlfn.CEILING.MATH(V17)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X17">
-        <f>COUNTIF(B17:U17,"&lt;"&amp;V17)/COUNT(B17:U17)*100</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="Y17">
-        <f>COUNTIF(B17:U17,"&gt;"&amp;V17)/COUNT(B17:U17)*100</f>
+        <f t="shared" si="3"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Z17">
-        <f>COUNTIF(B17:U17,"&lt;"&amp;W17)/COUNT(B17:U17)*100</f>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="AA17">
-        <f>COUNTIF(B17:U17,"&gt;"&amp;U17)/COUNT(B17:U17)*100</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
     </row>
@@ -5537,27 +5537,27 @@
         <v>4</v>
       </c>
       <c r="V18">
-        <f>AVERAGE(A18:U18)</f>
+        <f t="shared" si="0"/>
         <v>8.15</v>
       </c>
       <c r="W18">
-        <f>_xlfn.CEILING.MATH(V18)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X18">
-        <f>COUNTIF(B18:U18,"&lt;"&amp;V18)/COUNT(B18:U18)*100</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="Y18">
-        <f>COUNTIF(B18:U18,"&gt;"&amp;V18)/COUNT(B18:U18)*100</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="Z18">
-        <f>COUNTIF(B18:U18,"&lt;"&amp;W18)/COUNT(B18:U18)*100</f>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="AA18">
-        <f>COUNTIF(B18:U18,"&gt;"&amp;U18)/COUNT(B18:U18)*100</f>
+        <f t="shared" si="5"/>
         <v>95</v>
       </c>
     </row>
@@ -5626,27 +5626,27 @@
         <v>14</v>
       </c>
       <c r="V19">
-        <f>AVERAGE(A19:U19)</f>
+        <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
       <c r="W19">
-        <f>_xlfn.CEILING.MATH(V19)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X19">
-        <f>COUNTIF(B19:U19,"&lt;"&amp;V19)/COUNT(B19:U19)*100</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="Y19">
-        <f>COUNTIF(B19:U19,"&gt;"&amp;V19)/COUNT(B19:U19)*100</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="Z19">
-        <f>COUNTIF(B19:U19,"&lt;"&amp;W19)/COUNT(B19:U19)*100</f>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="AA19">
-        <f>COUNTIF(B19:U19,"&gt;"&amp;U19)/COUNT(B19:U19)*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5715,27 +5715,27 @@
         <v>8</v>
       </c>
       <c r="V20">
-        <f>AVERAGE(A20:U20)</f>
+        <f t="shared" si="0"/>
         <v>8.15</v>
       </c>
       <c r="W20">
-        <f>_xlfn.CEILING.MATH(V20)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X20">
-        <f>COUNTIF(B20:U20,"&lt;"&amp;V20)/COUNT(B20:U20)*100</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="Y20">
-        <f>COUNTIF(B20:U20,"&gt;"&amp;V20)/COUNT(B20:U20)*100</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="Z20">
-        <f>COUNTIF(B20:U20,"&lt;"&amp;W20)/COUNT(B20:U20)*100</f>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="AA20">
-        <f>COUNTIF(B20:U20,"&gt;"&amp;U20)/COUNT(B20:U20)*100</f>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
     </row>
@@ -5804,27 +5804,27 @@
         <v>9</v>
       </c>
       <c r="V21">
-        <f>AVERAGE(A21:U21)</f>
+        <f t="shared" si="0"/>
         <v>6.95</v>
       </c>
       <c r="W21">
-        <f>_xlfn.CEILING.MATH(V21)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="X21">
-        <f>COUNTIF(B21:U21,"&lt;"&amp;V21)/COUNT(B21:U21)*100</f>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="Y21">
-        <f>COUNTIF(B21:U21,"&gt;"&amp;V21)/COUNT(B21:U21)*100</f>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="Z21">
-        <f>COUNTIF(B21:U21,"&lt;"&amp;W21)/COUNT(B21:U21)*100</f>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="AA21">
-        <f>COUNTIF(B21:U21,"&gt;"&amp;U21)/COUNT(B21:U21)*100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5893,27 +5893,27 @@
         <v>10</v>
       </c>
       <c r="V22">
-        <f>AVERAGE(A22:U22)</f>
+        <f t="shared" si="0"/>
         <v>8.6999999999999993</v>
       </c>
       <c r="W22">
-        <f>_xlfn.CEILING.MATH(V22)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X22">
-        <f>COUNTIF(B22:U22,"&lt;"&amp;V22)/COUNT(B22:U22)*100</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="Y22">
-        <f>COUNTIF(B22:U22,"&gt;"&amp;V22)/COUNT(B22:U22)*100</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="Z22">
-        <f>COUNTIF(B22:U22,"&lt;"&amp;W22)/COUNT(B22:U22)*100</f>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="AA22">
-        <f>COUNTIF(B22:U22,"&gt;"&amp;U22)/COUNT(B22:U22)*100</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
@@ -5982,27 +5982,27 @@
         <v>8</v>
       </c>
       <c r="V23">
-        <f>AVERAGE(A23:U23)</f>
+        <f t="shared" si="0"/>
         <v>7.95</v>
       </c>
       <c r="W23">
-        <f>_xlfn.CEILING.MATH(V23)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="X23">
-        <f>COUNTIF(B23:U23,"&lt;"&amp;V23)/COUNT(B23:U23)*100</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="Y23">
-        <f>COUNTIF(B23:U23,"&gt;"&amp;V23)/COUNT(B23:U23)*100</f>
+        <f t="shared" si="3"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Z23">
-        <f>COUNTIF(B23:U23,"&lt;"&amp;W23)/COUNT(B23:U23)*100</f>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="AA23">
-        <f>COUNTIF(B23:U23,"&gt;"&amp;U23)/COUNT(B23:U23)*100</f>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
@@ -6071,27 +6071,27 @@
         <v>6</v>
       </c>
       <c r="V24">
-        <f>AVERAGE(A24:U24)</f>
+        <f t="shared" si="0"/>
         <v>7.15</v>
       </c>
       <c r="W24">
-        <f>_xlfn.CEILING.MATH(V24)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="X24">
-        <f>COUNTIF(B24:U24,"&lt;"&amp;V24)/COUNT(B24:U24)*100</f>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="Y24">
-        <f>COUNTIF(B24:U24,"&gt;"&amp;V24)/COUNT(B24:U24)*100</f>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="Z24">
-        <f>COUNTIF(B24:U24,"&lt;"&amp;W24)/COUNT(B24:U24)*100</f>
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
       <c r="AA24">
-        <f>COUNTIF(B24:U24,"&gt;"&amp;U24)/COUNT(B24:U24)*100</f>
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
     </row>
@@ -6160,27 +6160,27 @@
         <v>8</v>
       </c>
       <c r="V25">
-        <f>AVERAGE(A25:U25)</f>
+        <f t="shared" si="0"/>
         <v>7.55</v>
       </c>
       <c r="W25">
-        <f>_xlfn.CEILING.MATH(V25)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="X25">
-        <f>COUNTIF(B25:U25,"&lt;"&amp;V25)/COUNT(B25:U25)*100</f>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="Y25">
-        <f>COUNTIF(B25:U25,"&gt;"&amp;V25)/COUNT(B25:U25)*100</f>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="Z25">
-        <f>COUNTIF(B25:U25,"&lt;"&amp;W25)/COUNT(B25:U25)*100</f>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="AA25">
-        <f>COUNTIF(B25:U25,"&gt;"&amp;U25)/COUNT(B25:U25)*100</f>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
     </row>
@@ -6249,27 +6249,27 @@
         <v>10</v>
       </c>
       <c r="V26">
-        <f>AVERAGE(A26:U26)</f>
+        <f t="shared" si="0"/>
         <v>8.35</v>
       </c>
       <c r="W26">
-        <f>_xlfn.CEILING.MATH(V26)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X26">
-        <f>COUNTIF(B26:U26,"&lt;"&amp;V26)/COUNT(B26:U26)*100</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="Y26">
-        <f>COUNTIF(B26:U26,"&gt;"&amp;V26)/COUNT(B26:U26)*100</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="Z26">
-        <f>COUNTIF(B26:U26,"&lt;"&amp;W26)/COUNT(B26:U26)*100</f>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="AA26">
-        <f>COUNTIF(B26:U26,"&gt;"&amp;U26)/COUNT(B26:U26)*100</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
     </row>
@@ -6338,27 +6338,27 @@
         <v>6</v>
       </c>
       <c r="V27">
-        <f>AVERAGE(A27:U27)</f>
+        <f t="shared" si="0"/>
         <v>8.0500000000000007</v>
       </c>
       <c r="W27">
-        <f>_xlfn.CEILING.MATH(V27)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X27">
-        <f>COUNTIF(B27:U27,"&lt;"&amp;V27)/COUNT(B27:U27)*100</f>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="Y27">
-        <f>COUNTIF(B27:U27,"&gt;"&amp;V27)/COUNT(B27:U27)*100</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="Z27">
-        <f>COUNTIF(B27:U27,"&lt;"&amp;W27)/COUNT(B27:U27)*100</f>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="AA27">
-        <f>COUNTIF(B27:U27,"&gt;"&amp;U27)/COUNT(B27:U27)*100</f>
+        <f t="shared" si="5"/>
         <v>80</v>
       </c>
     </row>
@@ -6427,27 +6427,27 @@
         <v>9</v>
       </c>
       <c r="V28">
-        <f>AVERAGE(A28:U28)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="W28">
-        <f>_xlfn.CEILING.MATH(V28)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="X28">
-        <f>COUNTIF(B28:U28,"&lt;"&amp;V28)/COUNT(B28:U28)*100</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="Y28">
-        <f>COUNTIF(B28:U28,"&gt;"&amp;V28)/COUNT(B28:U28)*100</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="Z28">
-        <f>COUNTIF(B28:U28,"&lt;"&amp;W28)/COUNT(B28:U28)*100</f>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="AA28">
-        <f>COUNTIF(B28:U28,"&gt;"&amp;U28)/COUNT(B28:U28)*100</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
     </row>
@@ -6516,27 +6516,27 @@
         <v>8</v>
       </c>
       <c r="V29">
-        <f>AVERAGE(A29:U29)</f>
+        <f t="shared" si="0"/>
         <v>8.15</v>
       </c>
       <c r="W29">
-        <f>_xlfn.CEILING.MATH(V29)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X29">
-        <f>COUNTIF(B29:U29,"&lt;"&amp;V29)/COUNT(B29:U29)*100</f>
+        <f t="shared" si="2"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Y29">
-        <f>COUNTIF(B29:U29,"&gt;"&amp;V29)/COUNT(B29:U29)*100</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="Z29">
-        <f>COUNTIF(B29:U29,"&lt;"&amp;W29)/COUNT(B29:U29)*100</f>
+        <f t="shared" si="4"/>
         <v>55.000000000000007</v>
       </c>
       <c r="AA29">
-        <f>COUNTIF(B29:U29,"&gt;"&amp;U29)/COUNT(B29:U29)*100</f>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
@@ -6605,27 +6605,27 @@
         <v>5</v>
       </c>
       <c r="V30">
-        <f>AVERAGE(A30:U30)</f>
+        <f t="shared" si="0"/>
         <v>4.25</v>
       </c>
       <c r="W30">
-        <f>_xlfn.CEILING.MATH(V30)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="X30">
-        <f>COUNTIF(B30:U30,"&lt;"&amp;V30)/COUNT(B30:U30)*100</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="Y30">
-        <f>COUNTIF(B30:U30,"&gt;"&amp;V30)/COUNT(B30:U30)*100</f>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="Z30">
-        <f>COUNTIF(B30:U30,"&lt;"&amp;W30)/COUNT(B30:U30)*100</f>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="AA30">
-        <f>COUNTIF(B30:U30,"&gt;"&amp;U30)/COUNT(B30:U30)*100</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
     </row>
@@ -6694,27 +6694,27 @@
         <v>5</v>
       </c>
       <c r="V31">
-        <f>AVERAGE(A31:U31)</f>
+        <f t="shared" si="0"/>
         <v>3.85</v>
       </c>
       <c r="W31">
-        <f>_xlfn.CEILING.MATH(V31)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="X31">
-        <f>COUNTIF(B31:U31,"&lt;"&amp;V31)/COUNT(B31:U31)*100</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="Y31">
-        <f>COUNTIF(B31:U31,"&gt;"&amp;V31)/COUNT(B31:U31)*100</f>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="Z31">
-        <f>COUNTIF(B31:U31,"&lt;"&amp;W31)/COUNT(B31:U31)*100</f>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="AA31">
-        <f>COUNTIF(B31:U31,"&gt;"&amp;U31)/COUNT(B31:U31)*100</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
@@ -6783,27 +6783,27 @@
         <v>7</v>
       </c>
       <c r="V32">
-        <f>AVERAGE(A32:U32)</f>
+        <f t="shared" si="0"/>
         <v>8.25</v>
       </c>
       <c r="W32">
-        <f>_xlfn.CEILING.MATH(V32)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="X32">
-        <f>COUNTIF(B32:U32,"&lt;"&amp;V32)/COUNT(B32:U32)*100</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="Y32">
-        <f>COUNTIF(B32:U32,"&gt;"&amp;V32)/COUNT(B32:U32)*100</f>
+        <f t="shared" si="3"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Z32">
-        <f>COUNTIF(B32:U32,"&lt;"&amp;W32)/COUNT(B32:U32)*100</f>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="AA32">
-        <f>COUNTIF(B32:U32,"&gt;"&amp;U32)/COUNT(B32:U32)*100</f>
+        <f t="shared" si="5"/>
         <v>55.000000000000007</v>
       </c>
     </row>
@@ -6872,27 +6872,27 @@
         <v>8</v>
       </c>
       <c r="V33">
-        <f>AVERAGE(A33:U33)</f>
+        <f t="shared" si="0"/>
         <v>7.65</v>
       </c>
       <c r="W33">
-        <f>_xlfn.CEILING.MATH(V33)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="X33">
-        <f>COUNTIF(B33:U33,"&lt;"&amp;V33)/COUNT(B33:U33)*100</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="Y33">
-        <f>COUNTIF(B33:U33,"&gt;"&amp;V33)/COUNT(B33:U33)*100</f>
+        <f t="shared" si="3"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Z33">
-        <f>COUNTIF(B33:U33,"&lt;"&amp;W33)/COUNT(B33:U33)*100</f>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="AA33">
-        <f>COUNTIF(B33:U33,"&gt;"&amp;U33)/COUNT(B33:U33)*100</f>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
     </row>
@@ -6961,27 +6961,27 @@
         <v>10</v>
       </c>
       <c r="V34">
-        <f>AVERAGE(A34:U34)</f>
+        <f t="shared" ref="V34:V65" si="7">AVERAGE(A34:U34)</f>
         <v>8</v>
       </c>
       <c r="W34">
-        <f>_xlfn.CEILING.MATH(V34)</f>
+        <f t="shared" ref="W34:W65" si="8">_xlfn.CEILING.MATH(V34)</f>
         <v>8</v>
       </c>
       <c r="X34">
-        <f>COUNTIF(B34:U34,"&lt;"&amp;V34)/COUNT(B34:U34)*100</f>
+        <f t="shared" ref="X34:X66" si="9">COUNTIF(B34:U34,"&lt;"&amp;V34)/COUNT(B34:U34)*100</f>
         <v>40</v>
       </c>
       <c r="Y34">
-        <f>COUNTIF(B34:U34,"&gt;"&amp;V34)/COUNT(B34:U34)*100</f>
+        <f t="shared" ref="Y34:Y66" si="10">COUNTIF(B34:U34,"&gt;"&amp;V34)/COUNT(B34:U34)*100</f>
         <v>40</v>
       </c>
       <c r="Z34">
-        <f>COUNTIF(B34:U34,"&lt;"&amp;W34)/COUNT(B34:U34)*100</f>
+        <f t="shared" ref="Z34:Z66" si="11">COUNTIF(B34:U34,"&lt;"&amp;W34)/COUNT(B34:U34)*100</f>
         <v>40</v>
       </c>
       <c r="AA34">
-        <f>COUNTIF(B34:U34,"&gt;"&amp;U34)/COUNT(B34:U34)*100</f>
+        <f t="shared" ref="AA34:AA66" si="12">COUNTIF(B34:U34,"&gt;"&amp;U34)/COUNT(B34:U34)*100</f>
         <v>10</v>
       </c>
     </row>
@@ -7050,27 +7050,27 @@
         <v>9</v>
       </c>
       <c r="V35">
-        <f>AVERAGE(A35:U35)</f>
+        <f t="shared" si="7"/>
         <v>8.5500000000000007</v>
       </c>
       <c r="W35">
-        <f>_xlfn.CEILING.MATH(V35)</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="X35">
-        <f>COUNTIF(B35:U35,"&lt;"&amp;V35)/COUNT(B35:U35)*100</f>
+        <f t="shared" si="9"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Y35">
-        <f>COUNTIF(B35:U35,"&gt;"&amp;V35)/COUNT(B35:U35)*100</f>
+        <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="Z35">
-        <f>COUNTIF(B35:U35,"&lt;"&amp;W35)/COUNT(B35:U35)*100</f>
+        <f t="shared" si="11"/>
         <v>55.000000000000007</v>
       </c>
       <c r="AA35">
-        <f>COUNTIF(B35:U35,"&gt;"&amp;U35)/COUNT(B35:U35)*100</f>
+        <f t="shared" si="12"/>
         <v>25</v>
       </c>
     </row>
@@ -7139,27 +7139,27 @@
         <v>4</v>
       </c>
       <c r="V36">
-        <f>AVERAGE(A36:U36)</f>
+        <f t="shared" si="7"/>
         <v>7.5</v>
       </c>
       <c r="W36">
-        <f>_xlfn.CEILING.MATH(V36)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="X36">
-        <f>COUNTIF(B36:U36,"&lt;"&amp;V36)/COUNT(B36:U36)*100</f>
+        <f t="shared" si="9"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Y36">
-        <f>COUNTIF(B36:U36,"&gt;"&amp;V36)/COUNT(B36:U36)*100</f>
+        <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="Z36">
-        <f>COUNTIF(B36:U36,"&lt;"&amp;W36)/COUNT(B36:U36)*100</f>
+        <f t="shared" si="11"/>
         <v>55.000000000000007</v>
       </c>
       <c r="AA36">
-        <f>COUNTIF(B36:U36,"&gt;"&amp;U36)/COUNT(B36:U36)*100</f>
+        <f t="shared" si="12"/>
         <v>85</v>
       </c>
     </row>
@@ -7228,27 +7228,27 @@
         <v>10</v>
       </c>
       <c r="V37">
-        <f>AVERAGE(A37:U37)</f>
+        <f t="shared" si="7"/>
         <v>7.45</v>
       </c>
       <c r="W37">
-        <f>_xlfn.CEILING.MATH(V37)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="X37">
-        <f>COUNTIF(B37:U37,"&lt;"&amp;V37)/COUNT(B37:U37)*100</f>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="Y37">
-        <f>COUNTIF(B37:U37,"&gt;"&amp;V37)/COUNT(B37:U37)*100</f>
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
       <c r="Z37">
-        <f>COUNTIF(B37:U37,"&lt;"&amp;W37)/COUNT(B37:U37)*100</f>
+        <f t="shared" si="11"/>
         <v>60</v>
       </c>
       <c r="AA37">
-        <f>COUNTIF(B37:U37,"&gt;"&amp;U37)/COUNT(B37:U37)*100</f>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
     </row>
@@ -7317,27 +7317,27 @@
         <v>6</v>
       </c>
       <c r="V38">
-        <f>AVERAGE(A38:U38)</f>
+        <f t="shared" si="7"/>
         <v>7.9</v>
       </c>
       <c r="W38">
-        <f>_xlfn.CEILING.MATH(V38)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="X38">
-        <f>COUNTIF(B38:U38,"&lt;"&amp;V38)/COUNT(B38:U38)*100</f>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="Y38">
-        <f>COUNTIF(B38:U38,"&gt;"&amp;V38)/COUNT(B38:U38)*100</f>
+        <f t="shared" si="10"/>
         <v>60</v>
       </c>
       <c r="Z38">
-        <f>COUNTIF(B38:U38,"&lt;"&amp;W38)/COUNT(B38:U38)*100</f>
+        <f t="shared" si="11"/>
         <v>40</v>
       </c>
       <c r="AA38">
-        <f>COUNTIF(B38:U38,"&gt;"&amp;U38)/COUNT(B38:U38)*100</f>
+        <f t="shared" si="12"/>
         <v>65</v>
       </c>
     </row>
@@ -7406,27 +7406,27 @@
         <v>7</v>
       </c>
       <c r="V39">
-        <f>AVERAGE(A39:U39)</f>
+        <f t="shared" si="7"/>
         <v>7.7</v>
       </c>
       <c r="W39">
-        <f>_xlfn.CEILING.MATH(V39)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="X39">
-        <f>COUNTIF(B39:U39,"&lt;"&amp;V39)/COUNT(B39:U39)*100</f>
+        <f t="shared" si="9"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Y39">
-        <f>COUNTIF(B39:U39,"&gt;"&amp;V39)/COUNT(B39:U39)*100</f>
+        <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="Z39">
-        <f>COUNTIF(B39:U39,"&lt;"&amp;W39)/COUNT(B39:U39)*100</f>
+        <f t="shared" si="11"/>
         <v>55.000000000000007</v>
       </c>
       <c r="AA39">
-        <f>COUNTIF(B39:U39,"&gt;"&amp;U39)/COUNT(B39:U39)*100</f>
+        <f t="shared" si="12"/>
         <v>45</v>
       </c>
     </row>
@@ -7495,27 +7495,27 @@
         <v>8</v>
       </c>
       <c r="V40">
-        <f>AVERAGE(A40:U40)</f>
+        <f t="shared" si="7"/>
         <v>7.55</v>
       </c>
       <c r="W40">
-        <f>_xlfn.CEILING.MATH(V40)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="X40">
-        <f>COUNTIF(B40:U40,"&lt;"&amp;V40)/COUNT(B40:U40)*100</f>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="Y40">
-        <f>COUNTIF(B40:U40,"&gt;"&amp;V40)/COUNT(B40:U40)*100</f>
+        <f t="shared" si="10"/>
         <v>60</v>
       </c>
       <c r="Z40">
-        <f>COUNTIF(B40:U40,"&lt;"&amp;W40)/COUNT(B40:U40)*100</f>
+        <f t="shared" si="11"/>
         <v>40</v>
       </c>
       <c r="AA40">
-        <f>COUNTIF(B40:U40,"&gt;"&amp;U40)/COUNT(B40:U40)*100</f>
+        <f t="shared" si="12"/>
         <v>25</v>
       </c>
     </row>
@@ -7584,27 +7584,27 @@
         <v>10</v>
       </c>
       <c r="V41">
-        <f>AVERAGE(A41:U41)</f>
+        <f t="shared" si="7"/>
         <v>7.2</v>
       </c>
       <c r="W41">
-        <f>_xlfn.CEILING.MATH(V41)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="X41">
-        <f>COUNTIF(B41:U41,"&lt;"&amp;V41)/COUNT(B41:U41)*100</f>
+        <f t="shared" si="9"/>
         <v>65</v>
       </c>
       <c r="Y41">
-        <f>COUNTIF(B41:U41,"&gt;"&amp;V41)/COUNT(B41:U41)*100</f>
+        <f t="shared" si="10"/>
         <v>35</v>
       </c>
       <c r="Z41">
-        <f>COUNTIF(B41:U41,"&lt;"&amp;W41)/COUNT(B41:U41)*100</f>
+        <f t="shared" si="11"/>
         <v>65</v>
       </c>
       <c r="AA41">
-        <f>COUNTIF(B41:U41,"&gt;"&amp;U41)/COUNT(B41:U41)*100</f>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
     </row>
@@ -7673,27 +7673,27 @@
         <v>7</v>
       </c>
       <c r="V42">
-        <f>AVERAGE(A42:U42)</f>
+        <f t="shared" si="7"/>
         <v>8.75</v>
       </c>
       <c r="W42">
-        <f>_xlfn.CEILING.MATH(V42)</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="X42">
-        <f>COUNTIF(B42:U42,"&lt;"&amp;V42)/COUNT(B42:U42)*100</f>
+        <f t="shared" si="9"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Y42">
-        <f>COUNTIF(B42:U42,"&gt;"&amp;V42)/COUNT(B42:U42)*100</f>
+        <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="Z42">
-        <f>COUNTIF(B42:U42,"&lt;"&amp;W42)/COUNT(B42:U42)*100</f>
+        <f t="shared" si="11"/>
         <v>55.000000000000007</v>
       </c>
       <c r="AA42">
-        <f>COUNTIF(B42:U42,"&gt;"&amp;U42)/COUNT(B42:U42)*100</f>
+        <f t="shared" si="12"/>
         <v>65</v>
       </c>
     </row>
@@ -7762,27 +7762,27 @@
         <v>11</v>
       </c>
       <c r="V43">
-        <f>AVERAGE(A43:U43)</f>
+        <f t="shared" si="7"/>
         <v>8.65</v>
       </c>
       <c r="W43">
-        <f>_xlfn.CEILING.MATH(V43)</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="X43">
-        <f>COUNTIF(B43:U43,"&lt;"&amp;V43)/COUNT(B43:U43)*100</f>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="Y43">
-        <f>COUNTIF(B43:U43,"&gt;"&amp;V43)/COUNT(B43:U43)*100</f>
+        <f t="shared" si="10"/>
         <v>60</v>
       </c>
       <c r="Z43">
-        <f>COUNTIF(B43:U43,"&lt;"&amp;W43)/COUNT(B43:U43)*100</f>
+        <f t="shared" si="11"/>
         <v>40</v>
       </c>
       <c r="AA43">
-        <f>COUNTIF(B43:U43,"&gt;"&amp;U43)/COUNT(B43:U43)*100</f>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
     </row>
@@ -7851,27 +7851,27 @@
         <v>9</v>
       </c>
       <c r="V44">
-        <f>AVERAGE(A44:U44)</f>
+        <f t="shared" si="7"/>
         <v>8.1999999999999993</v>
       </c>
       <c r="W44">
-        <f>_xlfn.CEILING.MATH(V44)</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="X44">
-        <f>COUNTIF(B44:U44,"&lt;"&amp;V44)/COUNT(B44:U44)*100</f>
+        <f t="shared" si="9"/>
         <v>65</v>
       </c>
       <c r="Y44">
-        <f>COUNTIF(B44:U44,"&gt;"&amp;V44)/COUNT(B44:U44)*100</f>
+        <f t="shared" si="10"/>
         <v>35</v>
       </c>
       <c r="Z44">
-        <f>COUNTIF(B44:U44,"&lt;"&amp;W44)/COUNT(B44:U44)*100</f>
+        <f t="shared" si="11"/>
         <v>65</v>
       </c>
       <c r="AA44">
-        <f>COUNTIF(B44:U44,"&gt;"&amp;U44)/COUNT(B44:U44)*100</f>
+        <f t="shared" si="12"/>
         <v>25</v>
       </c>
     </row>
@@ -7940,27 +7940,27 @@
         <v>10</v>
       </c>
       <c r="V45">
-        <f>AVERAGE(A45:U45)</f>
+        <f t="shared" si="7"/>
         <v>8.5500000000000007</v>
       </c>
       <c r="W45">
-        <f>_xlfn.CEILING.MATH(V45)</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="X45">
-        <f>COUNTIF(B45:U45,"&lt;"&amp;V45)/COUNT(B45:U45)*100</f>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="Y45">
-        <f>COUNTIF(B45:U45,"&gt;"&amp;V45)/COUNT(B45:U45)*100</f>
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
       <c r="Z45">
-        <f>COUNTIF(B45:U45,"&lt;"&amp;W45)/COUNT(B45:U45)*100</f>
+        <f t="shared" si="11"/>
         <v>60</v>
       </c>
       <c r="AA45">
-        <f>COUNTIF(B45:U45,"&gt;"&amp;U45)/COUNT(B45:U45)*100</f>
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
     </row>
@@ -8029,27 +8029,27 @@
         <v>4</v>
       </c>
       <c r="V46">
-        <f>AVERAGE(A46:U46)</f>
+        <f t="shared" si="7"/>
         <v>7.2</v>
       </c>
       <c r="W46">
-        <f>_xlfn.CEILING.MATH(V46)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="X46">
-        <f>COUNTIF(B46:U46,"&lt;"&amp;V46)/COUNT(B46:U46)*100</f>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="Y46">
-        <f>COUNTIF(B46:U46,"&gt;"&amp;V46)/COUNT(B46:U46)*100</f>
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
       <c r="Z46">
-        <f>COUNTIF(B46:U46,"&lt;"&amp;W46)/COUNT(B46:U46)*100</f>
+        <f t="shared" si="11"/>
         <v>60</v>
       </c>
       <c r="AA46">
-        <f>COUNTIF(B46:U46,"&gt;"&amp;U46)/COUNT(B46:U46)*100</f>
+        <f t="shared" si="12"/>
         <v>90</v>
       </c>
     </row>
@@ -8118,27 +8118,27 @@
         <v>6</v>
       </c>
       <c r="V47">
-        <f>AVERAGE(A47:U47)</f>
+        <f t="shared" si="7"/>
         <v>7.05</v>
       </c>
       <c r="W47">
-        <f>_xlfn.CEILING.MATH(V47)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="X47">
-        <f>COUNTIF(B47:U47,"&lt;"&amp;V47)/COUNT(B47:U47)*100</f>
+        <f t="shared" si="9"/>
         <v>70</v>
       </c>
       <c r="Y47">
-        <f>COUNTIF(B47:U47,"&gt;"&amp;V47)/COUNT(B47:U47)*100</f>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="Z47">
-        <f>COUNTIF(B47:U47,"&lt;"&amp;W47)/COUNT(B47:U47)*100</f>
+        <f t="shared" si="11"/>
         <v>70</v>
       </c>
       <c r="AA47">
-        <f>COUNTIF(B47:U47,"&gt;"&amp;U47)/COUNT(B47:U47)*100</f>
+        <f t="shared" si="12"/>
         <v>40</v>
       </c>
     </row>
@@ -8207,27 +8207,27 @@
         <v>9</v>
       </c>
       <c r="V48">
-        <f>AVERAGE(A48:U48)</f>
+        <f t="shared" si="7"/>
         <v>8.5</v>
       </c>
       <c r="W48">
-        <f>_xlfn.CEILING.MATH(V48)</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="X48">
-        <f>COUNTIF(B48:U48,"&lt;"&amp;V48)/COUNT(B48:U48)*100</f>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="Y48">
-        <f>COUNTIF(B48:U48,"&gt;"&amp;V48)/COUNT(B48:U48)*100</f>
+        <f t="shared" si="10"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Z48">
-        <f>COUNTIF(B48:U48,"&lt;"&amp;W48)/COUNT(B48:U48)*100</f>
+        <f t="shared" si="11"/>
         <v>45</v>
       </c>
       <c r="AA48">
-        <f>COUNTIF(B48:U48,"&gt;"&amp;U48)/COUNT(B48:U48)*100</f>
+        <f t="shared" si="12"/>
         <v>35</v>
       </c>
     </row>
@@ -8296,27 +8296,27 @@
         <v>11</v>
       </c>
       <c r="V49">
-        <f>AVERAGE(A49:U49)</f>
+        <f t="shared" si="7"/>
         <v>8.1999999999999993</v>
       </c>
       <c r="W49">
-        <f>_xlfn.CEILING.MATH(V49)</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="X49">
-        <f>COUNTIF(B49:U49,"&lt;"&amp;V49)/COUNT(B49:U49)*100</f>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="Y49">
-        <f>COUNTIF(B49:U49,"&gt;"&amp;V49)/COUNT(B49:U49)*100</f>
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
       <c r="Z49">
-        <f>COUNTIF(B49:U49,"&lt;"&amp;W49)/COUNT(B49:U49)*100</f>
+        <f t="shared" si="11"/>
         <v>60</v>
       </c>
       <c r="AA49">
-        <f>COUNTIF(B49:U49,"&gt;"&amp;U49)/COUNT(B49:U49)*100</f>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
     </row>
@@ -8385,27 +8385,27 @@
         <v>5</v>
       </c>
       <c r="V50">
-        <f>AVERAGE(A50:U50)</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="W50">
-        <f>_xlfn.CEILING.MATH(V50)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="X50">
-        <f>COUNTIF(B50:U50,"&lt;"&amp;V50)/COUNT(B50:U50)*100</f>
+        <f t="shared" si="9"/>
         <v>35</v>
       </c>
       <c r="Y50">
-        <f>COUNTIF(B50:U50,"&gt;"&amp;V50)/COUNT(B50:U50)*100</f>
+        <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="Z50">
-        <f>COUNTIF(B50:U50,"&lt;"&amp;W50)/COUNT(B50:U50)*100</f>
+        <f t="shared" si="11"/>
         <v>35</v>
       </c>
       <c r="AA50">
-        <f>COUNTIF(B50:U50,"&gt;"&amp;U50)/COUNT(B50:U50)*100</f>
+        <f t="shared" si="12"/>
         <v>80</v>
       </c>
     </row>
@@ -8474,27 +8474,27 @@
         <v>12</v>
       </c>
       <c r="V51">
-        <f>AVERAGE(A51:U51)</f>
+        <f t="shared" si="7"/>
         <v>7.7</v>
       </c>
       <c r="W51">
-        <f>_xlfn.CEILING.MATH(V51)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="X51">
-        <f>COUNTIF(B51:U51,"&lt;"&amp;V51)/COUNT(B51:U51)*100</f>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="Y51">
-        <f>COUNTIF(B51:U51,"&gt;"&amp;V51)/COUNT(B51:U51)*100</f>
+        <f t="shared" si="10"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Z51">
-        <f>COUNTIF(B51:U51,"&lt;"&amp;W51)/COUNT(B51:U51)*100</f>
+        <f t="shared" si="11"/>
         <v>45</v>
       </c>
       <c r="AA51">
-        <f>COUNTIF(B51:U51,"&gt;"&amp;U51)/COUNT(B51:U51)*100</f>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
     </row>
@@ -8563,27 +8563,27 @@
         <v>12</v>
       </c>
       <c r="V52">
-        <f>AVERAGE(A52:U52)</f>
+        <f t="shared" si="7"/>
         <v>7.6</v>
       </c>
       <c r="W52">
-        <f>_xlfn.CEILING.MATH(V52)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="X52">
-        <f>COUNTIF(B52:U52,"&lt;"&amp;V52)/COUNT(B52:U52)*100</f>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="Y52">
-        <f>COUNTIF(B52:U52,"&gt;"&amp;V52)/COUNT(B52:U52)*100</f>
+        <f t="shared" si="10"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Z52">
-        <f>COUNTIF(B52:U52,"&lt;"&amp;W52)/COUNT(B52:U52)*100</f>
+        <f t="shared" si="11"/>
         <v>45</v>
       </c>
       <c r="AA52">
-        <f>COUNTIF(B52:U52,"&gt;"&amp;U52)/COUNT(B52:U52)*100</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -8652,27 +8652,27 @@
         <v>10</v>
       </c>
       <c r="V53">
-        <f>AVERAGE(A53:U53)</f>
+        <f t="shared" si="7"/>
         <v>7.9</v>
       </c>
       <c r="W53">
-        <f>_xlfn.CEILING.MATH(V53)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="X53">
-        <f>COUNTIF(B53:U53,"&lt;"&amp;V53)/COUNT(B53:U53)*100</f>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="Y53">
-        <f>COUNTIF(B53:U53,"&gt;"&amp;V53)/COUNT(B53:U53)*100</f>
+        <f t="shared" si="10"/>
         <v>60</v>
       </c>
       <c r="Z53">
-        <f>COUNTIF(B53:U53,"&lt;"&amp;W53)/COUNT(B53:U53)*100</f>
+        <f t="shared" si="11"/>
         <v>40</v>
       </c>
       <c r="AA53">
-        <f>COUNTIF(B53:U53,"&gt;"&amp;U53)/COUNT(B53:U53)*100</f>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
     </row>
@@ -8741,27 +8741,27 @@
         <v>8</v>
       </c>
       <c r="V54">
-        <f>AVERAGE(A54:U54)</f>
+        <f t="shared" si="7"/>
         <v>9.0500000000000007</v>
       </c>
       <c r="W54">
-        <f>_xlfn.CEILING.MATH(V54)</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="X54">
-        <f>COUNTIF(B54:U54,"&lt;"&amp;V54)/COUNT(B54:U54)*100</f>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="Y54">
-        <f>COUNTIF(B54:U54,"&gt;"&amp;V54)/COUNT(B54:U54)*100</f>
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
       <c r="Z54">
-        <f>COUNTIF(B54:U54,"&lt;"&amp;W54)/COUNT(B54:U54)*100</f>
+        <f t="shared" si="11"/>
         <v>60</v>
       </c>
       <c r="AA54">
-        <f>COUNTIF(B54:U54,"&gt;"&amp;U54)/COUNT(B54:U54)*100</f>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
     </row>
@@ -8830,27 +8830,27 @@
         <v>11</v>
       </c>
       <c r="V55">
-        <f>AVERAGE(A55:U55)</f>
+        <f t="shared" si="7"/>
         <v>9.4</v>
       </c>
       <c r="W55">
-        <f>_xlfn.CEILING.MATH(V55)</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="X55">
-        <f>COUNTIF(B55:U55,"&lt;"&amp;V55)/COUNT(B55:U55)*100</f>
+        <f t="shared" si="9"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Y55">
-        <f>COUNTIF(B55:U55,"&gt;"&amp;V55)/COUNT(B55:U55)*100</f>
+        <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="Z55">
-        <f>COUNTIF(B55:U55,"&lt;"&amp;W55)/COUNT(B55:U55)*100</f>
+        <f t="shared" si="11"/>
         <v>55.000000000000007</v>
       </c>
       <c r="AA55">
-        <f>COUNTIF(B55:U55,"&gt;"&amp;U55)/COUNT(B55:U55)*100</f>
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
     </row>
@@ -8919,27 +8919,27 @@
         <v>7</v>
       </c>
       <c r="V56">
-        <f>AVERAGE(A56:U56)</f>
+        <f t="shared" si="7"/>
         <v>8.15</v>
       </c>
       <c r="W56">
-        <f>_xlfn.CEILING.MATH(V56)</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="X56">
-        <f>COUNTIF(B56:U56,"&lt;"&amp;V56)/COUNT(B56:U56)*100</f>
+        <f t="shared" si="9"/>
         <v>65</v>
       </c>
       <c r="Y56">
-        <f>COUNTIF(B56:U56,"&gt;"&amp;V56)/COUNT(B56:U56)*100</f>
+        <f t="shared" si="10"/>
         <v>35</v>
       </c>
       <c r="Z56">
-        <f>COUNTIF(B56:U56,"&lt;"&amp;W56)/COUNT(B56:U56)*100</f>
+        <f t="shared" si="11"/>
         <v>65</v>
       </c>
       <c r="AA56">
-        <f>COUNTIF(B56:U56,"&gt;"&amp;U56)/COUNT(B56:U56)*100</f>
+        <f t="shared" si="12"/>
         <v>55.000000000000007</v>
       </c>
     </row>
@@ -9008,27 +9008,27 @@
         <v>3</v>
       </c>
       <c r="V57">
-        <f>AVERAGE(A57:U57)</f>
+        <f t="shared" si="7"/>
         <v>4.0999999999999996</v>
       </c>
       <c r="W57">
-        <f>_xlfn.CEILING.MATH(V57)</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="X57">
-        <f>COUNTIF(B57:U57,"&lt;"&amp;V57)/COUNT(B57:U57)*100</f>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="Y57">
-        <f>COUNTIF(B57:U57,"&gt;"&amp;V57)/COUNT(B57:U57)*100</f>
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
       <c r="Z57">
-        <f>COUNTIF(B57:U57,"&lt;"&amp;W57)/COUNT(B57:U57)*100</f>
+        <f t="shared" si="11"/>
         <v>60</v>
       </c>
       <c r="AA57">
-        <f>COUNTIF(B57:U57,"&gt;"&amp;U57)/COUNT(B57:U57)*100</f>
+        <f t="shared" si="12"/>
         <v>60</v>
       </c>
     </row>
@@ -9097,27 +9097,27 @@
         <v>3</v>
       </c>
       <c r="V58">
-        <f>AVERAGE(A58:U58)</f>
+        <f t="shared" si="7"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="W58">
-        <f>_xlfn.CEILING.MATH(V58)</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="X58">
-        <f>COUNTIF(B58:U58,"&lt;"&amp;V58)/COUNT(B58:U58)*100</f>
+        <f t="shared" si="9"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Y58">
-        <f>COUNTIF(B58:U58,"&gt;"&amp;V58)/COUNT(B58:U58)*100</f>
+        <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="Z58">
-        <f>COUNTIF(B58:U58,"&lt;"&amp;W58)/COUNT(B58:U58)*100</f>
+        <f t="shared" si="11"/>
         <v>55.000000000000007</v>
       </c>
       <c r="AA58">
-        <f>COUNTIF(B58:U58,"&gt;"&amp;U58)/COUNT(B58:U58)*100</f>
+        <f t="shared" si="12"/>
         <v>75</v>
       </c>
     </row>
@@ -9186,27 +9186,27 @@
         <v>3</v>
       </c>
       <c r="V59">
-        <f>AVERAGE(A59:U59)</f>
+        <f t="shared" si="7"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="W59">
-        <f>_xlfn.CEILING.MATH(V59)</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="X59">
-        <f>COUNTIF(B59:U59,"&lt;"&amp;V59)/COUNT(B59:U59)*100</f>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="Y59">
-        <f>COUNTIF(B59:U59,"&gt;"&amp;V59)/COUNT(B59:U59)*100</f>
+        <f t="shared" si="10"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Z59">
-        <f>COUNTIF(B59:U59,"&lt;"&amp;W59)/COUNT(B59:U59)*100</f>
+        <f t="shared" si="11"/>
         <v>45</v>
       </c>
       <c r="AA59">
-        <f>COUNTIF(B59:U59,"&gt;"&amp;U59)/COUNT(B59:U59)*100</f>
+        <f t="shared" si="12"/>
         <v>65</v>
       </c>
     </row>
@@ -9275,27 +9275,27 @@
         <v>3</v>
       </c>
       <c r="V60">
-        <f>AVERAGE(A60:U60)</f>
+        <f t="shared" si="7"/>
         <v>3.75</v>
       </c>
       <c r="W60">
-        <f>_xlfn.CEILING.MATH(V60)</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="X60">
-        <f>COUNTIF(B60:U60,"&lt;"&amp;V60)/COUNT(B60:U60)*100</f>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="Y60">
-        <f>COUNTIF(B60:U60,"&gt;"&amp;V60)/COUNT(B60:U60)*100</f>
+        <f t="shared" si="10"/>
         <v>60</v>
       </c>
       <c r="Z60">
-        <f>COUNTIF(B60:U60,"&lt;"&amp;W60)/COUNT(B60:U60)*100</f>
+        <f t="shared" si="11"/>
         <v>40</v>
       </c>
       <c r="AA60">
-        <f>COUNTIF(B60:U60,"&gt;"&amp;U60)/COUNT(B60:U60)*100</f>
+        <f t="shared" si="12"/>
         <v>60</v>
       </c>
     </row>
@@ -9364,27 +9364,27 @@
         <v>4</v>
       </c>
       <c r="V61">
-        <f>AVERAGE(A61:U61)</f>
+        <f t="shared" si="7"/>
         <v>4.75</v>
       </c>
       <c r="W61">
-        <f>_xlfn.CEILING.MATH(V61)</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="X61">
-        <f>COUNTIF(B61:U61,"&lt;"&amp;V61)/COUNT(B61:U61)*100</f>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="Y61">
-        <f>COUNTIF(B61:U61,"&gt;"&amp;V61)/COUNT(B61:U61)*100</f>
+        <f t="shared" si="10"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Z61">
-        <f>COUNTIF(B61:U61,"&lt;"&amp;W61)/COUNT(B61:U61)*100</f>
+        <f t="shared" si="11"/>
         <v>45</v>
       </c>
       <c r="AA61">
-        <f>COUNTIF(B61:U61,"&gt;"&amp;U61)/COUNT(B61:U61)*100</f>
+        <f t="shared" si="12"/>
         <v>55.000000000000007</v>
       </c>
     </row>
@@ -9453,27 +9453,27 @@
         <v>5</v>
       </c>
       <c r="V62">
-        <f>AVERAGE(A62:U62)</f>
+        <f t="shared" si="7"/>
         <v>4.45</v>
       </c>
       <c r="W62">
-        <f>_xlfn.CEILING.MATH(V62)</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="X62">
-        <f>COUNTIF(B62:U62,"&lt;"&amp;V62)/COUNT(B62:U62)*100</f>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="Y62">
-        <f>COUNTIF(B62:U62,"&gt;"&amp;V62)/COUNT(B62:U62)*100</f>
+        <f t="shared" si="10"/>
         <v>60</v>
       </c>
       <c r="Z62">
-        <f>COUNTIF(B62:U62,"&lt;"&amp;W62)/COUNT(B62:U62)*100</f>
+        <f t="shared" si="11"/>
         <v>40</v>
       </c>
       <c r="AA62">
-        <f>COUNTIF(B62:U62,"&gt;"&amp;U62)/COUNT(B62:U62)*100</f>
+        <f t="shared" si="12"/>
         <v>15</v>
       </c>
     </row>
@@ -9542,27 +9542,27 @@
         <v>3</v>
       </c>
       <c r="V63">
-        <f>AVERAGE(A63:U63)</f>
+        <f t="shared" si="7"/>
         <v>4.6500000000000004</v>
       </c>
       <c r="W63">
-        <f>_xlfn.CEILING.MATH(V63)</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="X63">
-        <f>COUNTIF(B63:U63,"&lt;"&amp;V63)/COUNT(B63:U63)*100</f>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="Y63">
-        <f>COUNTIF(B63:U63,"&gt;"&amp;V63)/COUNT(B63:U63)*100</f>
+        <f t="shared" si="10"/>
         <v>50</v>
       </c>
       <c r="Z63">
-        <f>COUNTIF(B63:U63,"&lt;"&amp;W63)/COUNT(B63:U63)*100</f>
+        <f t="shared" si="11"/>
         <v>50</v>
       </c>
       <c r="AA63">
-        <f>COUNTIF(B63:U63,"&gt;"&amp;U63)/COUNT(B63:U63)*100</f>
+        <f t="shared" si="12"/>
         <v>75</v>
       </c>
     </row>
@@ -9631,27 +9631,27 @@
         <v>7</v>
       </c>
       <c r="V64">
-        <f>AVERAGE(A64:U64)</f>
+        <f t="shared" si="7"/>
         <v>4.8499999999999996</v>
       </c>
       <c r="W64">
-        <f>_xlfn.CEILING.MATH(V64)</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="X64">
-        <f>COUNTIF(B64:U64,"&lt;"&amp;V64)/COUNT(B64:U64)*100</f>
+        <f t="shared" si="9"/>
         <v>35</v>
       </c>
       <c r="Y64">
-        <f>COUNTIF(B64:U64,"&gt;"&amp;V64)/COUNT(B64:U64)*100</f>
+        <f t="shared" si="10"/>
         <v>65</v>
       </c>
       <c r="Z64">
-        <f>COUNTIF(B64:U64,"&lt;"&amp;W64)/COUNT(B64:U64)*100</f>
+        <f t="shared" si="11"/>
         <v>35</v>
       </c>
       <c r="AA64">
-        <f>COUNTIF(B64:U64,"&gt;"&amp;U64)/COUNT(B64:U64)*100</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -9720,27 +9720,27 @@
         <v>6</v>
       </c>
       <c r="V65">
-        <f>AVERAGE(A65:U65)</f>
+        <f t="shared" si="7"/>
         <v>4.75</v>
       </c>
       <c r="W65">
-        <f>_xlfn.CEILING.MATH(V65)</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="X65">
-        <f>COUNTIF(B65:U65,"&lt;"&amp;V65)/COUNT(B65:U65)*100</f>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="Y65">
-        <f>COUNTIF(B65:U65,"&gt;"&amp;V65)/COUNT(B65:U65)*100</f>
+        <f t="shared" si="10"/>
         <v>55.000000000000007</v>
       </c>
       <c r="Z65">
-        <f>COUNTIF(B65:U65,"&lt;"&amp;W65)/COUNT(B65:U65)*100</f>
+        <f t="shared" si="11"/>
         <v>45</v>
       </c>
       <c r="AA65">
-        <f>COUNTIF(B65:U65,"&gt;"&amp;U65)/COUNT(B65:U65)*100</f>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
     </row>
@@ -9809,31 +9809,32 @@
         <v>5</v>
       </c>
       <c r="V66">
-        <f>AVERAGE(A66:U66)</f>
+        <f t="shared" ref="V66:V97" si="13">AVERAGE(A66:U66)</f>
         <v>4.3499999999999996</v>
       </c>
       <c r="W66">
-        <f>_xlfn.CEILING.MATH(V66)</f>
+        <f t="shared" ref="W66:W97" si="14">_xlfn.CEILING.MATH(V66)</f>
         <v>5</v>
       </c>
       <c r="X66">
-        <f>COUNTIF(B66:U66,"&lt;"&amp;V66)/COUNT(B66:U66)*100</f>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="Y66">
-        <f>COUNTIF(B66:U66,"&gt;"&amp;V66)/COUNT(B66:U66)*100</f>
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
       <c r="Z66">
-        <f>COUNTIF(B66:U66,"&lt;"&amp;W66)/COUNT(B66:U66)*100</f>
+        <f t="shared" si="11"/>
         <v>60</v>
       </c>
       <c r="AA66">
-        <f>COUNTIF(B66:U66,"&gt;"&amp;U66)/COUNT(B66:U66)*100</f>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>